<commit_message>
unit info in progress
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_unit_info.xlsx
+++ b/dbHelpers/generator_unit_info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BFB2CE-2593-4D68-BE37-BBAE3DD3AE4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -39,12 +40,21 @@
   </si>
   <si>
     <t>trial_run_date</t>
+  </si>
+  <si>
+    <t>Solapur</t>
+  </si>
+  <si>
+    <t>eminating_lines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,11 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,22 +369,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,11 +396,14 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -395,13 +411,51 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>800</v>
-      </c>
-      <c r="D2">
-        <v>1600</v>
+        <v>75</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43619</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>75</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43618</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43618</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change in excel
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_unit_info.xlsx
+++ b/dbHelpers/generator_unit_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3C0926-D42F-4B08-ACFC-9A14EB0F5437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5314E6DC-F2A5-412F-816D-9A7215238A78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Solapur</t>
-  </si>
-  <si>
-    <t>emanating_lines</t>
   </si>
 </sst>
 </file>
@@ -370,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,11 +379,10 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,11 +395,8 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -416,11 +409,8 @@
       <c r="D2" s="2">
         <v>43619</v>
       </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -433,11 +423,8 @@
       <c r="D3" s="2">
         <v>43618</v>
       </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -449,9 +436,6 @@
       </c>
       <c r="D4" s="2">
         <v>43618</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cod dates excel
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_unit_info.xlsx
+++ b/dbHelpers/generator_unit_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6254C5-5B3B-4138-91B2-96536A593BEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFF4F5B-8D26-449D-8E73-FF7C638D95BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
gadarwara trail run date
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_unit_info.xlsx
+++ b/dbHelpers/generator_unit_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D52161-292A-47A7-81BB-DE21491494C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F1B5BA-D45D-472F-AE6F-94285A35DD7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
         <v>75</v>
       </c>
       <c r="D2" s="2">
-        <v>43619</v>
+        <v>43424</v>
       </c>
       <c r="E2" s="3">
         <v>43617</v>

</xml_diff>